<commit_message>
Text overlay on Photo Edit begun
also some changes to specs doc, etc
</commit_message>
<xml_diff>
--- a/docs/Bugs and Issues.xlsx
+++ b/docs/Bugs and Issues.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
   <si>
     <t>Performance or Feature Issue</t>
   </si>
@@ -109,6 +109,18 @@
   </si>
   <si>
     <t>FIXED</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>in progress</t>
+  </si>
+  <si>
+    <t>complete</t>
+  </si>
+  <si>
+    <t>not yet begun</t>
   </si>
 </sst>
 </file>
@@ -176,9 +188,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,7 +495,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,13 +628,13 @@
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>30</v>
       </c>
     </row>
@@ -630,47 +642,81 @@
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
+      <c r="C16" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>